<commit_message>
corrections kth and added slu data 2020
</commit_message>
<xml_diff>
--- a/data/slu/original_data/slu_apc_2020_210531.xlsx
+++ b/data/slu/original_data/slu_apc_2020_210531.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage-al.slu.se\home$\dlal0002\My Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camlin\system\openapc-se\data\slu\original_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="190">
   <si>
     <t>institution</t>
   </si>
@@ -570,6 +570,30 @@
   </si>
   <si>
     <t>10.3390/su12125142</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>journal_full_title</t>
+  </si>
+  <si>
+    <t>issn</t>
+  </si>
+  <si>
+    <t>issn_print</t>
+  </si>
+  <si>
+    <t>issn_electronic</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
 </sst>
 </file>
@@ -625,7 +649,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -887,13 +911,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -909,8 +935,26 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -923,11 +967,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -940,11 +984,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -957,11 +1001,11 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -974,11 +1018,11 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -991,11 +1035,11 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1008,11 +1052,11 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1025,11 +1069,11 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1042,11 +1086,11 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1059,11 +1103,11 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1076,11 +1120,11 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1093,11 +1137,11 @@
       <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1110,11 +1154,11 @@
       <c r="D13" t="s">
         <v>17</v>
       </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1127,11 +1171,11 @@
       <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1144,11 +1188,11 @@
       <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1161,11 +1205,11 @@
       <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1178,11 +1222,11 @@
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1195,11 +1239,11 @@
       <c r="D18" t="s">
         <v>22</v>
       </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1212,11 +1256,11 @@
       <c r="D19" t="s">
         <v>23</v>
       </c>
-      <c r="E19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1229,11 +1273,11 @@
       <c r="D20" t="s">
         <v>24</v>
       </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1246,11 +1290,11 @@
       <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1263,11 +1307,11 @@
       <c r="D22" t="s">
         <v>26</v>
       </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1280,11 +1324,11 @@
       <c r="D23" t="s">
         <v>27</v>
       </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1297,11 +1341,11 @@
       <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="E24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1314,11 +1358,11 @@
       <c r="D25" t="s">
         <v>29</v>
       </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1331,11 +1375,11 @@
       <c r="D26" t="s">
         <v>30</v>
       </c>
-      <c r="E26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1348,11 +1392,11 @@
       <c r="D27" t="s">
         <v>31</v>
       </c>
-      <c r="E27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1365,11 +1409,11 @@
       <c r="D28" t="s">
         <v>32</v>
       </c>
-      <c r="E28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1382,11 +1426,11 @@
       <c r="D29" t="s">
         <v>33</v>
       </c>
-      <c r="E29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1399,11 +1443,11 @@
       <c r="D30" t="s">
         <v>34</v>
       </c>
-      <c r="E30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1416,11 +1460,11 @@
       <c r="D31" t="s">
         <v>35</v>
       </c>
-      <c r="E31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1433,11 +1477,11 @@
       <c r="D32" t="s">
         <v>36</v>
       </c>
-      <c r="E32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1450,11 +1494,11 @@
       <c r="D33" t="s">
         <v>37</v>
       </c>
-      <c r="E33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1467,11 +1511,11 @@
       <c r="D34" t="s">
         <v>38</v>
       </c>
-      <c r="E34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1484,11 +1528,11 @@
       <c r="D35" t="s">
         <v>39</v>
       </c>
-      <c r="E35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1501,11 +1545,11 @@
       <c r="D36" t="s">
         <v>40</v>
       </c>
-      <c r="E36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1518,11 +1562,11 @@
       <c r="D37" t="s">
         <v>41</v>
       </c>
-      <c r="E37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1535,11 +1579,11 @@
       <c r="D38" t="s">
         <v>42</v>
       </c>
-      <c r="E38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1552,11 +1596,11 @@
       <c r="D39" t="s">
         <v>43</v>
       </c>
-      <c r="E39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1569,11 +1613,11 @@
       <c r="D40" t="s">
         <v>44</v>
       </c>
-      <c r="E40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1586,11 +1630,11 @@
       <c r="D41" t="s">
         <v>45</v>
       </c>
-      <c r="E41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1603,11 +1647,11 @@
       <c r="D42" t="s">
         <v>46</v>
       </c>
-      <c r="E42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1620,11 +1664,11 @@
       <c r="D43" t="s">
         <v>47</v>
       </c>
-      <c r="E43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1637,11 +1681,11 @@
       <c r="D44" t="s">
         <v>48</v>
       </c>
-      <c r="E44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1654,11 +1698,11 @@
       <c r="D45" t="s">
         <v>49</v>
       </c>
-      <c r="E45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1671,11 +1715,11 @@
       <c r="D46" t="s">
         <v>50</v>
       </c>
-      <c r="E46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1688,11 +1732,11 @@
       <c r="D47" t="s">
         <v>51</v>
       </c>
-      <c r="E47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1705,11 +1749,11 @@
       <c r="D48" t="s">
         <v>52</v>
       </c>
-      <c r="E48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1722,11 +1766,11 @@
       <c r="D49" t="s">
         <v>53</v>
       </c>
-      <c r="E49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1739,11 +1783,11 @@
       <c r="D50" t="s">
         <v>54</v>
       </c>
-      <c r="E50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1756,11 +1800,11 @@
       <c r="D51" t="s">
         <v>55</v>
       </c>
-      <c r="E51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1773,11 +1817,11 @@
       <c r="D52" t="s">
         <v>56</v>
       </c>
-      <c r="E52" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1790,11 +1834,11 @@
       <c r="D53" t="s">
         <v>57</v>
       </c>
-      <c r="E53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1807,11 +1851,11 @@
       <c r="D54" t="s">
         <v>58</v>
       </c>
-      <c r="E54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -1824,11 +1868,11 @@
       <c r="D55" t="s">
         <v>59</v>
       </c>
-      <c r="E55" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1841,11 +1885,11 @@
       <c r="D56" t="s">
         <v>60</v>
       </c>
-      <c r="E56" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1858,11 +1902,11 @@
       <c r="D57" t="s">
         <v>61</v>
       </c>
-      <c r="E57" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1875,11 +1919,11 @@
       <c r="D58" t="s">
         <v>62</v>
       </c>
-      <c r="E58" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1892,11 +1936,11 @@
       <c r="D59" t="s">
         <v>63</v>
       </c>
-      <c r="E59" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1909,11 +1953,11 @@
       <c r="D60" t="s">
         <v>64</v>
       </c>
-      <c r="E60" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1926,11 +1970,11 @@
       <c r="D61" t="s">
         <v>65</v>
       </c>
-      <c r="E61" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -1943,11 +1987,11 @@
       <c r="D62" t="s">
         <v>66</v>
       </c>
-      <c r="E62" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -1960,11 +2004,11 @@
       <c r="D63" t="s">
         <v>67</v>
       </c>
-      <c r="E63" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -1977,11 +2021,11 @@
       <c r="D64" t="s">
         <v>68</v>
       </c>
-      <c r="E64" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1994,11 +2038,11 @@
       <c r="D65" t="s">
         <v>69</v>
       </c>
-      <c r="E65" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -2011,11 +2055,11 @@
       <c r="D66" t="s">
         <v>70</v>
       </c>
-      <c r="E66" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -2028,11 +2072,11 @@
       <c r="D67" t="s">
         <v>71</v>
       </c>
-      <c r="E67" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -2045,11 +2089,11 @@
       <c r="D68" t="s">
         <v>72</v>
       </c>
-      <c r="E68" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -2062,11 +2106,11 @@
       <c r="D69" t="s">
         <v>73</v>
       </c>
-      <c r="E69" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -2079,11 +2123,11 @@
       <c r="D70" t="s">
         <v>74</v>
       </c>
-      <c r="E70" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -2096,11 +2140,11 @@
       <c r="D71" t="s">
         <v>75</v>
       </c>
-      <c r="E71" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -2113,11 +2157,11 @@
       <c r="D72" t="s">
         <v>76</v>
       </c>
-      <c r="E72" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -2130,11 +2174,11 @@
       <c r="D73" t="s">
         <v>77</v>
       </c>
-      <c r="E73" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -2147,11 +2191,11 @@
       <c r="D74" t="s">
         <v>78</v>
       </c>
-      <c r="E74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -2164,11 +2208,11 @@
       <c r="D75" t="s">
         <v>79</v>
       </c>
-      <c r="E75" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -2181,11 +2225,11 @@
       <c r="D76" t="s">
         <v>80</v>
       </c>
-      <c r="E76" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -2198,11 +2242,11 @@
       <c r="D77" t="s">
         <v>81</v>
       </c>
-      <c r="E77" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -2215,11 +2259,11 @@
       <c r="D78" t="s">
         <v>82</v>
       </c>
-      <c r="E78" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -2232,11 +2276,11 @@
       <c r="D79" t="s">
         <v>83</v>
       </c>
-      <c r="E79" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -2249,11 +2293,11 @@
       <c r="D80" t="s">
         <v>84</v>
       </c>
-      <c r="E80" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -2266,11 +2310,11 @@
       <c r="D81" t="s">
         <v>85</v>
       </c>
-      <c r="E81" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -2283,11 +2327,11 @@
       <c r="D82" t="s">
         <v>86</v>
       </c>
-      <c r="E82" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -2300,11 +2344,11 @@
       <c r="D83" t="s">
         <v>87</v>
       </c>
-      <c r="E83" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -2317,11 +2361,11 @@
       <c r="D84" t="s">
         <v>88</v>
       </c>
-      <c r="E84" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -2334,11 +2378,11 @@
       <c r="D85" t="s">
         <v>89</v>
       </c>
-      <c r="E85" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -2351,11 +2395,11 @@
       <c r="D86" t="s">
         <v>90</v>
       </c>
-      <c r="E86" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -2368,11 +2412,11 @@
       <c r="D87" t="s">
         <v>91</v>
       </c>
-      <c r="E87" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -2385,11 +2429,11 @@
       <c r="D88" t="s">
         <v>92</v>
       </c>
-      <c r="E88" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -2402,11 +2446,11 @@
       <c r="D89" t="s">
         <v>93</v>
       </c>
-      <c r="E89" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -2419,11 +2463,11 @@
       <c r="D90" t="s">
         <v>94</v>
       </c>
-      <c r="E90" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -2436,11 +2480,11 @@
       <c r="D91" t="s">
         <v>95</v>
       </c>
-      <c r="E91" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -2453,11 +2497,11 @@
       <c r="D92" t="s">
         <v>96</v>
       </c>
-      <c r="E92" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -2470,11 +2514,11 @@
       <c r="D93" t="s">
         <v>97</v>
       </c>
-      <c r="E93" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -2487,11 +2531,11 @@
       <c r="D94" t="s">
         <v>98</v>
       </c>
-      <c r="E94" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -2504,11 +2548,11 @@
       <c r="D95" t="s">
         <v>99</v>
       </c>
-      <c r="E95" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>5</v>
       </c>
@@ -2521,11 +2565,11 @@
       <c r="D96" t="s">
         <v>100</v>
       </c>
-      <c r="E96" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -2538,11 +2582,11 @@
       <c r="D97" t="s">
         <v>101</v>
       </c>
-      <c r="E97" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>5</v>
       </c>
@@ -2555,11 +2599,11 @@
       <c r="D98" t="s">
         <v>102</v>
       </c>
-      <c r="E98" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -2572,11 +2616,11 @@
       <c r="D99" t="s">
         <v>103</v>
       </c>
-      <c r="E99" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>5</v>
       </c>
@@ -2589,11 +2633,11 @@
       <c r="D100" t="s">
         <v>104</v>
       </c>
-      <c r="E100" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>5</v>
       </c>
@@ -2606,11 +2650,11 @@
       <c r="D101" t="s">
         <v>105</v>
       </c>
-      <c r="E101" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -2623,11 +2667,11 @@
       <c r="D102" t="s">
         <v>106</v>
       </c>
-      <c r="E102" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -2640,11 +2684,11 @@
       <c r="D103" t="s">
         <v>107</v>
       </c>
-      <c r="E103" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>5</v>
       </c>
@@ -2657,11 +2701,11 @@
       <c r="D104" t="s">
         <v>108</v>
       </c>
-      <c r="E104" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E104" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>5</v>
       </c>
@@ -2674,11 +2718,11 @@
       <c r="D105" t="s">
         <v>109</v>
       </c>
-      <c r="E105" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>5</v>
       </c>
@@ -2691,11 +2735,11 @@
       <c r="D106" t="s">
         <v>110</v>
       </c>
-      <c r="E106" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E106" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -2708,11 +2752,11 @@
       <c r="D107" t="s">
         <v>111</v>
       </c>
-      <c r="E107" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E107" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>5</v>
       </c>
@@ -2725,11 +2769,11 @@
       <c r="D108" t="s">
         <v>112</v>
       </c>
-      <c r="E108" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E108" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>5</v>
       </c>
@@ -2742,11 +2786,11 @@
       <c r="D109" t="s">
         <v>113</v>
       </c>
-      <c r="E109" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>5</v>
       </c>
@@ -2759,11 +2803,11 @@
       <c r="D110" t="s">
         <v>114</v>
       </c>
-      <c r="E110" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E110" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -2776,11 +2820,11 @@
       <c r="D111" t="s">
         <v>115</v>
       </c>
-      <c r="E111" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E111" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -2793,11 +2837,11 @@
       <c r="D112" t="s">
         <v>116</v>
       </c>
-      <c r="E112" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E112" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>5</v>
       </c>
@@ -2810,11 +2854,11 @@
       <c r="D113" t="s">
         <v>117</v>
       </c>
-      <c r="E113" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>5</v>
       </c>
@@ -2827,11 +2871,11 @@
       <c r="D114" t="s">
         <v>118</v>
       </c>
-      <c r="E114" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E114" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>5</v>
       </c>
@@ -2844,11 +2888,11 @@
       <c r="D115" t="s">
         <v>119</v>
       </c>
-      <c r="E115" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E115" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -2861,11 +2905,11 @@
       <c r="D116" t="s">
         <v>120</v>
       </c>
-      <c r="E116" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>5</v>
       </c>
@@ -2878,11 +2922,11 @@
       <c r="D117" t="s">
         <v>121</v>
       </c>
-      <c r="E117" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>5</v>
       </c>
@@ -2895,11 +2939,11 @@
       <c r="D118" t="s">
         <v>122</v>
       </c>
-      <c r="E118" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E118" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>5</v>
       </c>
@@ -2912,11 +2956,11 @@
       <c r="D119" t="s">
         <v>123</v>
       </c>
-      <c r="E119" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E119" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>5</v>
       </c>
@@ -2929,11 +2973,11 @@
       <c r="D120" t="s">
         <v>124</v>
       </c>
-      <c r="E120" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E120" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>5</v>
       </c>
@@ -2946,11 +2990,11 @@
       <c r="D121" t="s">
         <v>125</v>
       </c>
-      <c r="E121" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E121" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>5</v>
       </c>
@@ -2963,11 +3007,11 @@
       <c r="D122" t="s">
         <v>126</v>
       </c>
-      <c r="E122" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E122" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>5</v>
       </c>
@@ -2980,11 +3024,11 @@
       <c r="D123" t="s">
         <v>127</v>
       </c>
-      <c r="E123" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E123" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>5</v>
       </c>
@@ -2997,11 +3041,11 @@
       <c r="D124" t="s">
         <v>128</v>
       </c>
-      <c r="E124" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>5</v>
       </c>
@@ -3014,11 +3058,11 @@
       <c r="D125" t="s">
         <v>129</v>
       </c>
-      <c r="E125" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>5</v>
       </c>
@@ -3031,11 +3075,11 @@
       <c r="D126" t="s">
         <v>130</v>
       </c>
-      <c r="E126" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E126" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>5</v>
       </c>
@@ -3048,11 +3092,11 @@
       <c r="D127" t="s">
         <v>131</v>
       </c>
-      <c r="E127" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E127" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>5</v>
       </c>
@@ -3065,11 +3109,11 @@
       <c r="D128" t="s">
         <v>132</v>
       </c>
-      <c r="E128" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E128" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>5</v>
       </c>
@@ -3082,11 +3126,11 @@
       <c r="D129" t="s">
         <v>133</v>
       </c>
-      <c r="E129" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E129" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>5</v>
       </c>
@@ -3099,11 +3143,11 @@
       <c r="D130" t="s">
         <v>134</v>
       </c>
-      <c r="E130" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>5</v>
       </c>
@@ -3116,11 +3160,11 @@
       <c r="D131" t="s">
         <v>135</v>
       </c>
-      <c r="E131" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>5</v>
       </c>
@@ -3133,11 +3177,11 @@
       <c r="D132" t="s">
         <v>136</v>
       </c>
-      <c r="E132" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E132" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>5</v>
       </c>
@@ -3150,11 +3194,11 @@
       <c r="D133" t="s">
         <v>137</v>
       </c>
-      <c r="E133" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>5</v>
       </c>
@@ -3167,11 +3211,11 @@
       <c r="D134" t="s">
         <v>138</v>
       </c>
-      <c r="E134" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E134" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>5</v>
       </c>
@@ -3184,11 +3228,11 @@
       <c r="D135" t="s">
         <v>139</v>
       </c>
-      <c r="E135" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E135" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>5</v>
       </c>
@@ -3201,11 +3245,11 @@
       <c r="D136" t="s">
         <v>140</v>
       </c>
-      <c r="E136" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E136" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>5</v>
       </c>
@@ -3218,11 +3262,11 @@
       <c r="D137" t="s">
         <v>141</v>
       </c>
-      <c r="E137" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>5</v>
       </c>
@@ -3235,11 +3279,11 @@
       <c r="D138" t="s">
         <v>142</v>
       </c>
-      <c r="E138" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E138" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>5</v>
       </c>
@@ -3252,11 +3296,11 @@
       <c r="D139" t="s">
         <v>143</v>
       </c>
-      <c r="E139" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E139" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>5</v>
       </c>
@@ -3269,11 +3313,11 @@
       <c r="D140" t="s">
         <v>144</v>
       </c>
-      <c r="E140" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E140" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>5</v>
       </c>
@@ -3286,11 +3330,11 @@
       <c r="D141" t="s">
         <v>145</v>
       </c>
-      <c r="E141" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E141" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>5</v>
       </c>
@@ -3303,11 +3347,11 @@
       <c r="D142" t="s">
         <v>146</v>
       </c>
-      <c r="E142" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E142" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>5</v>
       </c>
@@ -3320,11 +3364,11 @@
       <c r="D143" t="s">
         <v>147</v>
       </c>
-      <c r="E143" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E143" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>5</v>
       </c>
@@ -3337,11 +3381,11 @@
       <c r="D144" t="s">
         <v>148</v>
       </c>
-      <c r="E144" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>5</v>
       </c>
@@ -3354,11 +3398,11 @@
       <c r="D145" t="s">
         <v>149</v>
       </c>
-      <c r="E145" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E145" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>5</v>
       </c>
@@ -3371,11 +3415,11 @@
       <c r="D146" t="s">
         <v>150</v>
       </c>
-      <c r="E146" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E146" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -3388,11 +3432,11 @@
       <c r="D147" t="s">
         <v>151</v>
       </c>
-      <c r="E147" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E147" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>5</v>
       </c>
@@ -3405,11 +3449,11 @@
       <c r="D148" t="s">
         <v>152</v>
       </c>
-      <c r="E148" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E148" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>5</v>
       </c>
@@ -3422,11 +3466,11 @@
       <c r="D149" t="s">
         <v>153</v>
       </c>
-      <c r="E149" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E149" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>5</v>
       </c>
@@ -3439,11 +3483,11 @@
       <c r="D150" t="s">
         <v>154</v>
       </c>
-      <c r="E150" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E150" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>5</v>
       </c>
@@ -3456,11 +3500,11 @@
       <c r="D151" t="s">
         <v>155</v>
       </c>
-      <c r="E151" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>5</v>
       </c>
@@ -3473,11 +3517,11 @@
       <c r="D152" t="s">
         <v>156</v>
       </c>
-      <c r="E152" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E152" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>5</v>
       </c>
@@ -3490,11 +3534,11 @@
       <c r="D153" t="s">
         <v>157</v>
       </c>
-      <c r="E153" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E153" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>5</v>
       </c>
@@ -3507,11 +3551,11 @@
       <c r="D154" t="s">
         <v>158</v>
       </c>
-      <c r="E154" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E154" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>5</v>
       </c>
@@ -3524,11 +3568,11 @@
       <c r="D155" t="s">
         <v>159</v>
       </c>
-      <c r="E155" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E155" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>5</v>
       </c>
@@ -3541,11 +3585,11 @@
       <c r="D156" t="s">
         <v>160</v>
       </c>
-      <c r="E156" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E156" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>5</v>
       </c>
@@ -3558,11 +3602,11 @@
       <c r="D157" t="s">
         <v>161</v>
       </c>
-      <c r="E157" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E157" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>5</v>
       </c>
@@ -3575,11 +3619,11 @@
       <c r="D158" t="s">
         <v>162</v>
       </c>
-      <c r="E158" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E158" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>5</v>
       </c>
@@ -3592,11 +3636,11 @@
       <c r="D159" t="s">
         <v>163</v>
       </c>
-      <c r="E159" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E159" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>5</v>
       </c>
@@ -3609,11 +3653,11 @@
       <c r="D160" t="s">
         <v>164</v>
       </c>
-      <c r="E160" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E160" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>5</v>
       </c>
@@ -3626,11 +3670,11 @@
       <c r="D161" t="s">
         <v>165</v>
       </c>
-      <c r="E161" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E161" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>5</v>
       </c>
@@ -3643,11 +3687,11 @@
       <c r="D162" t="s">
         <v>166</v>
       </c>
-      <c r="E162" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E162" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>5</v>
       </c>
@@ -3660,11 +3704,11 @@
       <c r="D163" t="s">
         <v>167</v>
       </c>
-      <c r="E163" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E163" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>5</v>
       </c>
@@ -3677,11 +3721,11 @@
       <c r="D164" t="s">
         <v>168</v>
       </c>
-      <c r="E164" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E164" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>5</v>
       </c>
@@ -3694,11 +3738,11 @@
       <c r="D165" t="s">
         <v>169</v>
       </c>
-      <c r="E165" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E165" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>5</v>
       </c>
@@ -3711,11 +3755,11 @@
       <c r="D166" t="s">
         <v>170</v>
       </c>
-      <c r="E166" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E166" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>5</v>
       </c>
@@ -3728,11 +3772,11 @@
       <c r="D167" t="s">
         <v>171</v>
       </c>
-      <c r="E167" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E167" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>5</v>
       </c>
@@ -3745,11 +3789,11 @@
       <c r="D168" t="s">
         <v>172</v>
       </c>
-      <c r="E168" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E168" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>5</v>
       </c>
@@ -3762,11 +3806,11 @@
       <c r="D169" t="s">
         <v>173</v>
       </c>
-      <c r="E169" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E169" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>5</v>
       </c>
@@ -3779,11 +3823,11 @@
       <c r="D170" t="s">
         <v>174</v>
       </c>
-      <c r="E170" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E170" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>5</v>
       </c>
@@ -3796,11 +3840,11 @@
       <c r="D171" t="s">
         <v>175</v>
       </c>
-      <c r="E171" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E171" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>5</v>
       </c>
@@ -3813,11 +3857,11 @@
       <c r="D172" t="s">
         <v>176</v>
       </c>
-      <c r="E172" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E172" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>5</v>
       </c>
@@ -3830,11 +3874,11 @@
       <c r="D173" t="s">
         <v>177</v>
       </c>
-      <c r="E173" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E173" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>5</v>
       </c>
@@ -3847,11 +3891,11 @@
       <c r="D174" t="s">
         <v>178</v>
       </c>
-      <c r="E174" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E174" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>5</v>
       </c>
@@ -3864,11 +3908,11 @@
       <c r="D175" t="s">
         <v>179</v>
       </c>
-      <c r="E175" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E175" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>5</v>
       </c>
@@ -3881,11 +3925,11 @@
       <c r="D176" t="s">
         <v>180</v>
       </c>
-      <c r="E176" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E176" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>5</v>
       </c>
@@ -3898,8 +3942,8 @@
       <c r="D177" t="s">
         <v>181</v>
       </c>
-      <c r="E177" t="b">
-        <v>0</v>
+      <c r="E177" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>